<commit_message>
Added files for funds
</commit_message>
<xml_diff>
--- a/parameters/input_file_template.xlsx
+++ b/parameters/input_file_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_README" sheetId="6" r:id="rId1"/>
@@ -1107,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
@@ -1177,15 +1177,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" style="2"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>